<commit_message>
Negative words and Polarity Score done
</commit_message>
<xml_diff>
--- a/Output Data Structure.xlsx
+++ b/Output Data Structure.xlsx
@@ -487,8 +487,12 @@
       <c r="C2" s="2" t="n">
         <v>83</v>
       </c>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="2" t="n"/>
+      <c r="D2" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0.4954954910315721</v>
+      </c>
       <c r="F2" s="2" t="n"/>
       <c r="G2" s="2" t="n"/>
       <c r="H2" s="2" t="n"/>
@@ -525,8 +529,12 @@
       <c r="C3" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="n"/>
-      <c r="E3" s="2" t="n"/>
+      <c r="D3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.7647058373702448</v>
+      </c>
       <c r="F3" s="2" t="n"/>
       <c r="G3" s="2" t="n"/>
       <c r="H3" s="2" t="n"/>
@@ -563,8 +571,12 @@
       <c r="C4" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="n"/>
-      <c r="E4" s="2" t="n"/>
+      <c r="D4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.7142856802721105</v>
+      </c>
       <c r="F4" s="2" t="n"/>
       <c r="G4" s="2" t="n"/>
       <c r="H4" s="2" t="n"/>
@@ -601,8 +613,12 @@
       <c r="C5" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="n"/>
-      <c r="E5" s="2" t="n"/>
+      <c r="D5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.636363578512402</v>
+      </c>
       <c r="F5" s="2" t="n"/>
       <c r="G5" s="2" t="n"/>
       <c r="H5" s="2" t="n"/>
@@ -639,12 +655,12 @@
       <c r="C6" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n"/>
+      <c r="D6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.7999999200000081</v>
+      </c>
       <c r="F6" s="2" t="n"/>
       <c r="G6" s="2" t="n"/>
       <c r="H6" s="2" t="n"/>
@@ -681,8 +697,12 @@
       <c r="C7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="n"/>
-      <c r="E7" s="2" t="n"/>
+      <c r="D7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.09090908264462885</v>
+      </c>
       <c r="F7" s="2" t="n"/>
       <c r="G7" s="2" t="n"/>
       <c r="H7" s="2" t="n"/>
@@ -719,8 +739,12 @@
       <c r="C8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="n"/>
-      <c r="E8" s="2" t="n"/>
+      <c r="D8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0.7499999062500118</v>
+      </c>
       <c r="F8" s="2" t="n"/>
       <c r="G8" s="2" t="n"/>
       <c r="H8" s="2" t="n"/>
@@ -757,8 +781,12 @@
       <c r="C9" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="n"/>
-      <c r="E9" s="2" t="n"/>
+      <c r="D9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0.4999999375000079</v>
+      </c>
       <c r="F9" s="2" t="n"/>
       <c r="G9" s="2" t="n"/>
       <c r="H9" s="2" t="n"/>
@@ -795,8 +823,12 @@
       <c r="C10" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="2" t="n"/>
-      <c r="E10" s="2" t="n"/>
+      <c r="D10" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>-0.09090908264462885</v>
+      </c>
       <c r="F10" s="2" t="n"/>
       <c r="G10" s="2" t="n"/>
       <c r="H10" s="2" t="n"/>
@@ -833,8 +865,12 @@
       <c r="C11" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="n"/>
-      <c r="E11" s="2" t="n"/>
+      <c r="D11" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.5714285510204089</v>
+      </c>
       <c r="F11" s="2" t="n"/>
       <c r="G11" s="2" t="n"/>
       <c r="H11" s="2" t="n"/>
@@ -871,8 +907,12 @@
       <c r="C12" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="D12" s="2" t="n"/>
-      <c r="E12" s="2" t="n"/>
+      <c r="D12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.6969696758494038</v>
+      </c>
       <c r="F12" s="2" t="n"/>
       <c r="G12" s="2" t="n"/>
       <c r="H12" s="2" t="n"/>
@@ -909,8 +949,12 @@
       <c r="C13" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="D13" s="2" t="n"/>
-      <c r="E13" s="2" t="n"/>
+      <c r="D13" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0.4545454338842984</v>
+      </c>
       <c r="F13" s="2" t="n"/>
       <c r="G13" s="2" t="n"/>
       <c r="H13" s="2" t="n"/>
@@ -947,8 +991,12 @@
       <c r="C14" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="D14" s="2" t="n"/>
-      <c r="E14" s="2" t="n"/>
+      <c r="D14" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.799999960000002</v>
+      </c>
       <c r="F14" s="2" t="n"/>
       <c r="G14" s="2" t="n"/>
       <c r="H14" s="2" t="n"/>
@@ -985,8 +1033,12 @@
       <c r="C15" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="D15" s="2" t="n"/>
-      <c r="E15" s="2" t="n"/>
+      <c r="D15" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0.6551723912009521</v>
+      </c>
       <c r="F15" s="2" t="n"/>
       <c r="G15" s="2" t="n"/>
       <c r="H15" s="2" t="n"/>
@@ -1023,8 +1075,12 @@
       <c r="C16" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="D16" s="2" t="n"/>
-      <c r="E16" s="2" t="n"/>
+      <c r="D16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0.8333332986111125</v>
+      </c>
       <c r="F16" s="2" t="n"/>
       <c r="G16" s="2" t="n"/>
       <c r="H16" s="2" t="n"/>
@@ -1061,8 +1117,12 @@
       <c r="C17" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="D17" s="2" t="n"/>
-      <c r="E17" s="2" t="n"/>
+      <c r="D17" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0.7714285493877557</v>
+      </c>
       <c r="F17" s="2" t="n"/>
       <c r="G17" s="2" t="n"/>
       <c r="H17" s="2" t="n"/>
@@ -1099,8 +1159,12 @@
       <c r="C18" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="D18" s="2" t="n"/>
-      <c r="E18" s="2" t="n"/>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0.9999999411764739</v>
+      </c>
       <c r="F18" s="2" t="n"/>
       <c r="G18" s="2" t="n"/>
       <c r="H18" s="2" t="n"/>
@@ -1137,8 +1201,12 @@
       <c r="C19" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D19" s="2" t="n"/>
-      <c r="E19" s="2" t="n"/>
+      <c r="D19" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0.7037036776406045</v>
+      </c>
       <c r="F19" s="2" t="n"/>
       <c r="G19" s="2" t="n"/>
       <c r="H19" s="2" t="n"/>
@@ -1175,8 +1243,12 @@
       <c r="C20" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="D20" s="2" t="n"/>
-      <c r="E20" s="2" t="n"/>
+      <c r="D20" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0.6888888735802473</v>
+      </c>
       <c r="F20" s="2" t="n"/>
       <c r="G20" s="2" t="n"/>
       <c r="H20" s="2" t="n"/>
@@ -1213,8 +1285,12 @@
       <c r="C21" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="D21" s="2" t="n"/>
-      <c r="E21" s="2" t="n"/>
+      <c r="D21" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0.6874999785156257</v>
+      </c>
       <c r="F21" s="2" t="n"/>
       <c r="G21" s="2" t="n"/>
       <c r="H21" s="2" t="n"/>
@@ -1251,8 +1327,12 @@
       <c r="C22" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="D22" s="2" t="n"/>
-      <c r="E22" s="2" t="n"/>
+      <c r="D22" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0.7777777489711944</v>
+      </c>
       <c r="F22" s="2" t="n"/>
       <c r="G22" s="2" t="n"/>
       <c r="H22" s="2" t="n"/>
@@ -1289,8 +1369,12 @@
       <c r="C23" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D23" s="2" t="n"/>
-      <c r="E23" s="2" t="n"/>
+      <c r="D23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.9999996666667778</v>
+      </c>
       <c r="F23" s="2" t="n"/>
       <c r="G23" s="2" t="n"/>
       <c r="H23" s="2" t="n"/>
@@ -1327,8 +1411,12 @@
       <c r="C24" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D24" s="2" t="n"/>
-      <c r="E24" s="2" t="n"/>
+      <c r="D24" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.4999999583333368</v>
+      </c>
       <c r="F24" s="2" t="n"/>
       <c r="G24" s="2" t="n"/>
       <c r="H24" s="2" t="n"/>
@@ -1365,8 +1453,12 @@
       <c r="C25" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="D25" s="2" t="n"/>
-      <c r="E25" s="2" t="n"/>
+      <c r="D25" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.5999999828571434</v>
+      </c>
       <c r="F25" s="2" t="n"/>
       <c r="G25" s="2" t="n"/>
       <c r="H25" s="2" t="n"/>
@@ -1403,8 +1495,12 @@
       <c r="C26" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D26" s="2" t="n"/>
-      <c r="E26" s="2" t="n"/>
+      <c r="D26" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.4705882214532877</v>
+      </c>
       <c r="F26" s="2" t="n"/>
       <c r="G26" s="2" t="n"/>
       <c r="H26" s="2" t="n"/>
@@ -1441,8 +1537,12 @@
       <c r="C27" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="D27" s="2" t="n"/>
-      <c r="E27" s="2" t="n"/>
+      <c r="D27" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0.5483870790842877</v>
+      </c>
       <c r="F27" s="2" t="n"/>
       <c r="G27" s="2" t="n"/>
       <c r="H27" s="2" t="n"/>
@@ -1479,8 +1579,12 @@
       <c r="C28" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="D28" s="2" t="n"/>
-      <c r="E28" s="2" t="n"/>
+      <c r="D28" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0.1874999941406252</v>
+      </c>
       <c r="F28" s="2" t="n"/>
       <c r="G28" s="2" t="n"/>
       <c r="H28" s="2" t="n"/>
@@ -1517,8 +1621,12 @@
       <c r="C29" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D29" s="2" t="n"/>
-      <c r="E29" s="2" t="n"/>
+      <c r="D29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>0.7142856122449125</v>
+      </c>
       <c r="F29" s="2" t="n"/>
       <c r="G29" s="2" t="n"/>
       <c r="H29" s="2" t="n"/>
@@ -1555,8 +1663,12 @@
       <c r="C30" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D30" s="2" t="n"/>
-      <c r="E30" s="2" t="n"/>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>0.9999998333333611</v>
+      </c>
       <c r="F30" s="2" t="n"/>
       <c r="G30" s="2" t="n"/>
       <c r="H30" s="2" t="n"/>
@@ -1593,8 +1705,12 @@
       <c r="C31" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D31" s="2" t="n"/>
-      <c r="E31" s="2" t="n"/>
+      <c r="D31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>0.9999997500000625</v>
+      </c>
       <c r="F31" s="2" t="n"/>
       <c r="G31" s="2" t="n"/>
       <c r="H31" s="2" t="n"/>
@@ -1631,8 +1747,12 @@
       <c r="C32" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D32" s="2" t="n"/>
-      <c r="E32" s="2" t="n"/>
+      <c r="D32" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>0.599999880000024</v>
+      </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="2" t="n"/>
       <c r="H32" s="2" t="n"/>
@@ -1669,8 +1789,12 @@
       <c r="C33" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D33" s="2" t="n"/>
-      <c r="E33" s="2" t="n"/>
+      <c r="D33" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>0.6666665555555741</v>
+      </c>
       <c r="F33" s="2" t="n"/>
       <c r="G33" s="2" t="n"/>
       <c r="H33" s="2" t="n"/>
@@ -1707,8 +1831,12 @@
       <c r="C34" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D34" s="2" t="n"/>
-      <c r="E34" s="2" t="n"/>
+      <c r="D34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>0.99999980000004</v>
+      </c>
       <c r="F34" s="2" t="n"/>
       <c r="G34" s="2" t="n"/>
       <c r="H34" s="2" t="n"/>
@@ -1745,8 +1873,12 @@
       <c r="C35" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D35" s="2" t="n"/>
-      <c r="E35" s="2" t="n"/>
+      <c r="D35" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>0.7999999200000081</v>
+      </c>
       <c r="F35" s="2" t="n"/>
       <c r="G35" s="2" t="n"/>
       <c r="H35" s="2" t="n"/>
@@ -1783,8 +1915,12 @@
       <c r="C36" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D36" s="2" t="n"/>
-      <c r="E36" s="2" t="n"/>
+      <c r="D36" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>0.3333332962963004</v>
+      </c>
       <c r="F36" s="2" t="n"/>
       <c r="G36" s="2" t="n"/>
       <c r="H36" s="2" t="n"/>
@@ -1821,8 +1957,12 @@
       <c r="C37" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D37" s="2" t="n"/>
-      <c r="E37" s="2" t="n"/>
+      <c r="D37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>0.9999997500000625</v>
+      </c>
       <c r="F37" s="2" t="n"/>
       <c r="G37" s="2" t="n"/>
       <c r="H37" s="2" t="n"/>
@@ -1859,8 +1999,12 @@
       <c r="C38" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="D38" s="2" t="n"/>
-      <c r="E38" s="2" t="n"/>
+      <c r="D38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>0.9999999090909174</v>
+      </c>
       <c r="F38" s="2" t="n"/>
       <c r="G38" s="2" t="n"/>
       <c r="H38" s="2" t="n"/>
@@ -1897,8 +2041,12 @@
       <c r="C39" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D39" s="2" t="n"/>
-      <c r="E39" s="2" t="n"/>
+      <c r="D39" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>0.6666665555555741</v>
+      </c>
       <c r="F39" s="2" t="n"/>
       <c r="G39" s="2" t="n"/>
       <c r="H39" s="2" t="n"/>
@@ -1935,8 +2083,12 @@
       <c r="C40" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D40" s="2" t="n"/>
-      <c r="E40" s="2" t="n"/>
+      <c r="D40" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>0.4285713979591859</v>
+      </c>
       <c r="F40" s="2" t="n"/>
       <c r="G40" s="2" t="n"/>
       <c r="H40" s="2" t="n"/>
@@ -1973,8 +2125,12 @@
       <c r="C41" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D41" s="2" t="n"/>
-      <c r="E41" s="2" t="n"/>
+      <c r="D41" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>0.7999999200000081</v>
+      </c>
       <c r="F41" s="2" t="n"/>
       <c r="G41" s="2" t="n"/>
       <c r="H41" s="2" t="n"/>
@@ -2011,8 +2167,12 @@
       <c r="C42" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D42" s="2" t="n"/>
-      <c r="E42" s="2" t="n"/>
+      <c r="D42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>0.3333333111111126</v>
+      </c>
       <c r="F42" s="2" t="n"/>
       <c r="G42" s="2" t="n"/>
       <c r="H42" s="2" t="n"/>
@@ -2049,8 +2209,12 @@
       <c r="C43" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D43" s="2" t="n"/>
-      <c r="E43" s="2" t="n"/>
+      <c r="D43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>0.9999999166666736</v>
+      </c>
       <c r="F43" s="2" t="n"/>
       <c r="G43" s="2" t="n"/>
       <c r="H43" s="2" t="n"/>
@@ -2087,8 +2251,12 @@
       <c r="C44" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D44" s="2" t="n"/>
-      <c r="E44" s="2" t="n"/>
+      <c r="D44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>0.9999998750000157</v>
+      </c>
       <c r="F44" s="2" t="n"/>
       <c r="G44" s="2" t="n"/>
       <c r="H44" s="2" t="n"/>
@@ -2125,8 +2293,12 @@
       <c r="C45" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D45" s="2" t="n"/>
-      <c r="E45" s="2" t="n"/>
+      <c r="D45" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>0.5999999600000027</v>
+      </c>
       <c r="F45" s="2" t="n"/>
       <c r="G45" s="2" t="n"/>
       <c r="H45" s="2" t="n"/>
@@ -2163,8 +2335,12 @@
       <c r="C46" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="D46" s="2" t="n"/>
-      <c r="E46" s="2" t="n"/>
+      <c r="D46" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>0.4782608487712674</v>
+      </c>
       <c r="F46" s="2" t="n"/>
       <c r="G46" s="2" t="n"/>
       <c r="H46" s="2" t="n"/>
@@ -2201,8 +2377,12 @@
       <c r="C47" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="D47" s="2" t="n"/>
-      <c r="E47" s="2" t="n"/>
+      <c r="D47" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>0.5833333090277788</v>
+      </c>
       <c r="F47" s="2" t="n"/>
       <c r="G47" s="2" t="n"/>
       <c r="H47" s="2" t="n"/>
@@ -2239,8 +2419,12 @@
       <c r="C48" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D48" s="2" t="n"/>
-      <c r="E48" s="2" t="n"/>
+      <c r="D48" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>0.636363578512402</v>
+      </c>
       <c r="F48" s="2" t="n"/>
       <c r="G48" s="2" t="n"/>
       <c r="H48" s="2" t="n"/>
@@ -2277,8 +2461,12 @@
       <c r="C49" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D49" s="2" t="n"/>
-      <c r="E49" s="2" t="n"/>
+      <c r="D49" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>0.4117646816609011</v>
+      </c>
       <c r="F49" s="2" t="n"/>
       <c r="G49" s="2" t="n"/>
       <c r="H49" s="2" t="n"/>
@@ -2315,8 +2503,12 @@
       <c r="C50" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="D50" s="2" t="n"/>
-      <c r="E50" s="2" t="n"/>
+      <c r="D50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>0.2380952267573701</v>
+      </c>
       <c r="F50" s="2" t="n"/>
       <c r="G50" s="2" t="n"/>
       <c r="H50" s="2" t="n"/>
@@ -2353,8 +2545,12 @@
       <c r="C51" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D51" s="2" t="n"/>
-      <c r="E51" s="2" t="n"/>
+      <c r="D51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>0.9999998571428775</v>
+      </c>
       <c r="F51" s="2" t="n"/>
       <c r="G51" s="2" t="n"/>
       <c r="H51" s="2" t="n"/>
@@ -2391,8 +2587,12 @@
       <c r="C52" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D52" s="2" t="n"/>
-      <c r="E52" s="2" t="n"/>
+      <c r="D52" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>0.599999940000006</v>
+      </c>
       <c r="F52" s="2" t="n"/>
       <c r="G52" s="2" t="n"/>
       <c r="H52" s="2" t="n"/>
@@ -2429,8 +2629,12 @@
       <c r="C53" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="D53" s="2" t="n"/>
-      <c r="E53" s="2" t="n"/>
+      <c r="D53" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>0.5294117335640156</v>
+      </c>
       <c r="F53" s="2" t="n"/>
       <c r="G53" s="2" t="n"/>
       <c r="H53" s="2" t="n"/>
@@ -2467,8 +2671,12 @@
       <c r="C54" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="D54" s="2" t="n"/>
-      <c r="E54" s="2" t="n"/>
+      <c r="D54" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>0.2222222098765439</v>
+      </c>
       <c r="F54" s="2" t="n"/>
       <c r="G54" s="2" t="n"/>
       <c r="H54" s="2" t="n"/>
@@ -2505,8 +2713,12 @@
       <c r="C55" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D55" s="2" t="n"/>
-      <c r="E55" s="2" t="n"/>
+      <c r="D55" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>0.1428571224489825</v>
+      </c>
       <c r="F55" s="2" t="n"/>
       <c r="G55" s="2" t="n"/>
       <c r="H55" s="2" t="n"/>
@@ -2543,8 +2755,12 @@
       <c r="C56" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D56" s="2" t="n"/>
-      <c r="E56" s="2" t="n"/>
+      <c r="D56" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>0.7142856122449125</v>
+      </c>
       <c r="F56" s="2" t="n"/>
       <c r="G56" s="2" t="n"/>
       <c r="H56" s="2" t="n"/>
@@ -2581,8 +2797,12 @@
       <c r="C57" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D57" s="2" t="n"/>
-      <c r="E57" s="2" t="n"/>
+      <c r="D57" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>0.2307692130177529</v>
+      </c>
       <c r="F57" s="2" t="n"/>
       <c r="G57" s="2" t="n"/>
       <c r="H57" s="2" t="n"/>
@@ -2619,8 +2839,12 @@
       <c r="C58" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="D58" s="2" t="n"/>
-      <c r="E58" s="2" t="n"/>
+      <c r="D58" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>0.5294117335640156</v>
+      </c>
       <c r="F58" s="2" t="n"/>
       <c r="G58" s="2" t="n"/>
       <c r="H58" s="2" t="n"/>
@@ -2657,8 +2881,12 @@
       <c r="C59" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D59" s="2" t="n"/>
-      <c r="E59" s="2" t="n"/>
+      <c r="D59" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>0.7999999200000081</v>
+      </c>
       <c r="F59" s="2" t="n"/>
       <c r="G59" s="2" t="n"/>
       <c r="H59" s="2" t="n"/>
@@ -2695,8 +2923,12 @@
       <c r="C60" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D60" s="2" t="n"/>
-      <c r="E60" s="2" t="n"/>
+      <c r="D60" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>0.1428571224489825</v>
+      </c>
       <c r="F60" s="2" t="n"/>
       <c r="G60" s="2" t="n"/>
       <c r="H60" s="2" t="n"/>
@@ -2733,8 +2965,12 @@
       <c r="C61" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D61" s="2" t="n"/>
-      <c r="E61" s="2" t="n"/>
+      <c r="D61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>0.9999997500000625</v>
+      </c>
       <c r="F61" s="2" t="n"/>
       <c r="G61" s="2" t="n"/>
       <c r="H61" s="2" t="n"/>
@@ -2771,8 +3007,12 @@
       <c r="C62" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D62" s="2" t="n"/>
-      <c r="E62" s="2" t="n"/>
+      <c r="D62" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E62" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F62" s="2" t="n"/>
       <c r="G62" s="2" t="n"/>
       <c r="H62" s="2" t="n"/>
@@ -2809,8 +3049,12 @@
       <c r="C63" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D63" s="2" t="n"/>
-      <c r="E63" s="2" t="n"/>
+      <c r="D63" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2" t="n">
+        <v>0.7142856122449125</v>
+      </c>
       <c r="F63" s="2" t="n"/>
       <c r="G63" s="2" t="n"/>
       <c r="H63" s="2" t="n"/>
@@ -2847,8 +3091,12 @@
       <c r="C64" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D64" s="2" t="n"/>
-      <c r="E64" s="2" t="n"/>
+      <c r="D64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>0.99999980000004</v>
+      </c>
       <c r="F64" s="2" t="n"/>
       <c r="G64" s="2" t="n"/>
       <c r="H64" s="2" t="n"/>
@@ -2885,8 +3133,12 @@
       <c r="C65" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D65" s="2" t="n"/>
-      <c r="E65" s="2" t="n"/>
+      <c r="D65" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E65" s="2" t="n">
+        <v>0.1111110987654335</v>
+      </c>
       <c r="F65" s="2" t="n"/>
       <c r="G65" s="2" t="n"/>
       <c r="H65" s="2" t="n"/>
@@ -2923,8 +3175,12 @@
       <c r="C66" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="D66" s="2" t="n"/>
-      <c r="E66" s="2" t="n"/>
+      <c r="D66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>0.9999999090909174</v>
+      </c>
       <c r="F66" s="2" t="n"/>
       <c r="G66" s="2" t="n"/>
       <c r="H66" s="2" t="n"/>
@@ -2961,8 +3217,12 @@
       <c r="C67" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="D67" s="2" t="n"/>
-      <c r="E67" s="2" t="n"/>
+      <c r="D67" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>0.6470587854671302</v>
+      </c>
       <c r="F67" s="2" t="n"/>
       <c r="G67" s="2" t="n"/>
       <c r="H67" s="2" t="n"/>
@@ -2999,8 +3259,12 @@
       <c r="C68" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D68" s="2" t="n"/>
-      <c r="E68" s="2" t="n"/>
+      <c r="D68" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>0.2727272479338866</v>
+      </c>
       <c r="F68" s="2" t="n"/>
       <c r="G68" s="2" t="n"/>
       <c r="H68" s="2" t="n"/>
@@ -3037,8 +3301,12 @@
       <c r="C69" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D69" s="2" t="n"/>
-      <c r="E69" s="2" t="n"/>
+      <c r="D69" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>0.1538461479289943</v>
+      </c>
       <c r="F69" s="2" t="n"/>
       <c r="G69" s="2" t="n"/>
       <c r="H69" s="2" t="n"/>
@@ -3075,8 +3343,12 @@
       <c r="C70" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D70" s="2" t="n"/>
-      <c r="E70" s="2" t="n"/>
+      <c r="D70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>0.9999998571428775</v>
+      </c>
       <c r="F70" s="2" t="n"/>
       <c r="G70" s="2" t="n"/>
       <c r="H70" s="2" t="n"/>
@@ -3113,8 +3385,12 @@
       <c r="C71" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D71" s="2" t="n"/>
-      <c r="E71" s="2" t="n"/>
+      <c r="D71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>0.9999998750000157</v>
+      </c>
       <c r="F71" s="2" t="n"/>
       <c r="G71" s="2" t="n"/>
       <c r="H71" s="2" t="n"/>
@@ -3151,8 +3427,12 @@
       <c r="C72" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D72" s="2" t="n"/>
-      <c r="E72" s="2" t="n"/>
+      <c r="D72" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E72" s="2" t="n">
+        <v>0.7037036776406045</v>
+      </c>
       <c r="F72" s="2" t="n"/>
       <c r="G72" s="2" t="n"/>
       <c r="H72" s="2" t="n"/>
@@ -3189,8 +3469,12 @@
       <c r="C73" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D73" s="2" t="n"/>
-      <c r="E73" s="2" t="n"/>
+      <c r="D73" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E73" s="2" t="n">
+        <v>0.4999999583333368</v>
+      </c>
       <c r="F73" s="2" t="n"/>
       <c r="G73" s="2" t="n"/>
       <c r="H73" s="2" t="n"/>
@@ -3227,8 +3511,12 @@
       <c r="C74" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D74" s="2" t="n"/>
-      <c r="E74" s="2" t="n"/>
+      <c r="D74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2" t="n">
+        <v>0.9999998571428775</v>
+      </c>
       <c r="F74" s="2" t="n"/>
       <c r="G74" s="2" t="n"/>
       <c r="H74" s="2" t="n"/>
@@ -3265,8 +3553,12 @@
       <c r="C75" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D75" s="2" t="n"/>
-      <c r="E75" s="2" t="n"/>
+      <c r="D75" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E75" s="2" t="n">
+        <v>0.199999960000008</v>
+      </c>
       <c r="F75" s="2" t="n"/>
       <c r="G75" s="2" t="n"/>
       <c r="H75" s="2" t="n"/>
@@ -3303,8 +3595,12 @@
       <c r="C76" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D76" s="2" t="n"/>
-      <c r="E76" s="2" t="n"/>
+      <c r="D76" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E76" s="2" t="n">
+        <v>0.636363578512402</v>
+      </c>
       <c r="F76" s="2" t="n"/>
       <c r="G76" s="2" t="n"/>
       <c r="H76" s="2" t="n"/>
@@ -3341,8 +3637,12 @@
       <c r="C77" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D77" s="2" t="n"/>
-      <c r="E77" s="2" t="n"/>
+      <c r="D77" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E77" s="2" t="n">
+        <v>0.6666666111111158</v>
+      </c>
       <c r="F77" s="2" t="n"/>
       <c r="G77" s="2" t="n"/>
       <c r="H77" s="2" t="n"/>
@@ -3379,8 +3679,12 @@
       <c r="C78" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D78" s="2" t="n"/>
-      <c r="E78" s="2" t="n"/>
+      <c r="D78" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>0.3333332962963004</v>
+      </c>
       <c r="F78" s="2" t="n"/>
       <c r="G78" s="2" t="n"/>
       <c r="H78" s="2" t="n"/>
@@ -3417,8 +3721,12 @@
       <c r="C79" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D79" s="2" t="n"/>
-      <c r="E79" s="2" t="n"/>
+      <c r="D79" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="E79" s="2" t="n">
+        <v>-0.2999999850000007</v>
+      </c>
       <c r="F79" s="2" t="n"/>
       <c r="G79" s="2" t="n"/>
       <c r="H79" s="2" t="n"/>
@@ -3455,8 +3763,12 @@
       <c r="C80" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D80" s="2" t="n"/>
-      <c r="E80" s="2" t="n"/>
+      <c r="D80" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E80" s="2" t="n">
+        <v>-0.8333332638888947</v>
+      </c>
       <c r="F80" s="2" t="n"/>
       <c r="G80" s="2" t="n"/>
       <c r="H80" s="2" t="n"/>
@@ -3493,8 +3805,12 @@
       <c r="C81" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D81" s="2" t="n"/>
-      <c r="E81" s="2" t="n"/>
+      <c r="D81" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="n">
+        <v>0.599999880000024</v>
+      </c>
       <c r="F81" s="2" t="n"/>
       <c r="G81" s="2" t="n"/>
       <c r="H81" s="2" t="n"/>
@@ -3531,8 +3847,12 @@
       <c r="C82" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D82" s="2" t="n"/>
-      <c r="E82" s="2" t="n"/>
+      <c r="D82" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E82" s="2" t="n">
+        <v>-0.199999960000008</v>
+      </c>
       <c r="F82" s="2" t="n"/>
       <c r="G82" s="2" t="n"/>
       <c r="H82" s="2" t="n"/>
@@ -3569,8 +3889,12 @@
       <c r="C83" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="D83" s="2" t="n"/>
-      <c r="E83" s="2" t="n"/>
+      <c r="D83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="n">
+        <v>0.9999998750000157</v>
+      </c>
       <c r="F83" s="2" t="n"/>
       <c r="G83" s="2" t="n"/>
       <c r="H83" s="2" t="n"/>
@@ -3607,8 +3931,12 @@
       <c r="C84" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D84" s="2" t="n"/>
-      <c r="E84" s="2" t="n"/>
+      <c r="D84" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>0.166666652777779</v>
+      </c>
       <c r="F84" s="2" t="n"/>
       <c r="G84" s="2" t="n"/>
       <c r="H84" s="2" t="n"/>
@@ -3645,8 +3973,12 @@
       <c r="C85" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D85" s="2" t="n"/>
-      <c r="E85" s="2" t="n"/>
+      <c r="D85" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>0.5999999600000027</v>
+      </c>
       <c r="F85" s="2" t="n"/>
       <c r="G85" s="2" t="n"/>
       <c r="H85" s="2" t="n"/>
@@ -3683,8 +4015,12 @@
       <c r="C86" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D86" s="2" t="n"/>
-      <c r="E86" s="2" t="n"/>
+      <c r="D86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>0.99999950000025</v>
+      </c>
       <c r="F86" s="2" t="n"/>
       <c r="G86" s="2" t="n"/>
       <c r="H86" s="2" t="n"/>
@@ -3721,8 +4057,12 @@
       <c r="C87" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D87" s="2" t="n"/>
-      <c r="E87" s="2" t="n"/>
+      <c r="D87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>0.99999980000004</v>
+      </c>
       <c r="F87" s="2" t="n"/>
       <c r="G87" s="2" t="n"/>
       <c r="H87" s="2" t="n"/>
@@ -3759,8 +4099,12 @@
       <c r="C88" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D88" s="2" t="n"/>
-      <c r="E88" s="2" t="n"/>
+      <c r="D88" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>0.199999960000008</v>
+      </c>
       <c r="F88" s="2" t="n"/>
       <c r="G88" s="2" t="n"/>
       <c r="H88" s="2" t="n"/>
@@ -3797,8 +4141,12 @@
       <c r="C89" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D89" s="2" t="n"/>
-      <c r="E89" s="2" t="n"/>
+      <c r="D89" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>0.599999880000024</v>
+      </c>
       <c r="F89" s="2" t="n"/>
       <c r="G89" s="2" t="n"/>
       <c r="H89" s="2" t="n"/>
@@ -3835,8 +4183,12 @@
       <c r="C90" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D90" s="2" t="n"/>
-      <c r="E90" s="2" t="n"/>
+      <c r="D90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>0.9999990000010001</v>
+      </c>
       <c r="F90" s="2" t="n"/>
       <c r="G90" s="2" t="n"/>
       <c r="H90" s="2" t="n"/>
@@ -3873,8 +4225,12 @@
       <c r="C91" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D91" s="2" t="n"/>
-      <c r="E91" s="2" t="n"/>
+      <c r="D91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>0.9999998571428775</v>
+      </c>
       <c r="F91" s="2" t="n"/>
       <c r="G91" s="2" t="n"/>
       <c r="H91" s="2" t="n"/>
@@ -3911,8 +4267,12 @@
       <c r="C92" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D92" s="2" t="n"/>
-      <c r="E92" s="2" t="n"/>
+      <c r="D92" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>-0.2307692130177529</v>
+      </c>
       <c r="F92" s="2" t="n"/>
       <c r="G92" s="2" t="n"/>
       <c r="H92" s="2" t="n"/>
@@ -3949,8 +4309,12 @@
       <c r="C93" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="D93" s="2" t="n"/>
-      <c r="E93" s="2" t="n"/>
+      <c r="D93" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>0.8709677138397511</v>
+      </c>
       <c r="F93" s="2" t="n"/>
       <c r="G93" s="2" t="n"/>
       <c r="H93" s="2" t="n"/>
@@ -3987,8 +4351,12 @@
       <c r="C94" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="D94" s="2" t="n"/>
-      <c r="E94" s="2" t="n"/>
+      <c r="D94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>0.9999999677419364</v>
+      </c>
       <c r="F94" s="2" t="n"/>
       <c r="G94" s="2" t="n"/>
       <c r="H94" s="2" t="n"/>
@@ -4025,8 +4393,12 @@
       <c r="C95" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D95" s="2" t="n"/>
-      <c r="E95" s="2" t="n"/>
+      <c r="D95" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F95" s="2" t="n"/>
       <c r="G95" s="2" t="n"/>
       <c r="H95" s="2" t="n"/>
@@ -4063,8 +4435,12 @@
       <c r="C96" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="D96" s="2" t="n"/>
-      <c r="E96" s="2" t="n"/>
+      <c r="D96" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>0.7499999062500118</v>
+      </c>
       <c r="F96" s="2" t="n"/>
       <c r="G96" s="2" t="n"/>
       <c r="H96" s="2" t="n"/>
@@ -4101,8 +4477,12 @@
       <c r="C97" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="D97" s="2" t="n"/>
-      <c r="E97" s="2" t="n"/>
+      <c r="D97" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>0.636363578512402</v>
+      </c>
       <c r="F97" s="2" t="n"/>
       <c r="G97" s="2" t="n"/>
       <c r="H97" s="2" t="n"/>
@@ -4139,8 +4519,12 @@
       <c r="C98" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D98" s="2" t="n"/>
-      <c r="E98" s="2" t="n"/>
+      <c r="D98" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>-0.1111110987654335</v>
+      </c>
       <c r="F98" s="2" t="n"/>
       <c r="G98" s="2" t="n"/>
       <c r="H98" s="2" t="n"/>
@@ -4177,8 +4561,12 @@
       <c r="C99" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D99" s="2" t="n"/>
-      <c r="E99" s="2" t="n"/>
+      <c r="D99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>0.9999997500000625</v>
+      </c>
       <c r="F99" s="2" t="n"/>
       <c r="G99" s="2" t="n"/>
       <c r="H99" s="2" t="n"/>
@@ -4215,8 +4603,12 @@
       <c r="C100" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D100" s="2" t="n"/>
-      <c r="E100" s="2" t="n"/>
+      <c r="D100" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>0.7142856122449125</v>
+      </c>
       <c r="F100" s="2" t="n"/>
       <c r="G100" s="2" t="n"/>
       <c r="H100" s="2" t="n"/>
@@ -4253,8 +4645,12 @@
       <c r="C101" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D101" s="2" t="n"/>
-      <c r="E101" s="2" t="n"/>
+      <c r="D101" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2" t="n">
+        <v>0.6666665555555741</v>
+      </c>
       <c r="F101" s="2" t="n"/>
       <c r="G101" s="2" t="n"/>
       <c r="H101" s="2" t="n"/>
@@ -4291,6 +4687,12 @@
       <c r="C102" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="D102" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.4285713673469475</v>
+      </c>
     </row>
     <row r="103" ht="14.25" customHeight="1" s="8">
       <c r="A103" s="6" t="inlineStr">
@@ -4306,6 +4708,12 @@
       <c r="C103" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D103" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E103" t="n">
+        <v>-0.3333332222222593</v>
+      </c>
     </row>
     <row r="104" ht="14.25" customHeight="1" s="8">
       <c r="A104" s="6" t="inlineStr">
@@ -4321,6 +4729,12 @@
       <c r="C104" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="D104" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.399999960000004</v>
+      </c>
     </row>
     <row r="105" ht="14.25" customHeight="1" s="8">
       <c r="A105" s="6" t="inlineStr">
@@ -4336,6 +4750,12 @@
       <c r="C105" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="D105" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.99999980000004</v>
+      </c>
     </row>
     <row r="106" ht="14.25" customHeight="1" s="8">
       <c r="A106" s="6" t="inlineStr">
@@ -4351,6 +4771,12 @@
       <c r="C106" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="D106" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.8947368185595574</v>
+      </c>
     </row>
     <row r="107" ht="14.25" customHeight="1" s="8">
       <c r="A107" s="6" t="inlineStr">
@@ -4366,6 +4792,12 @@
       <c r="C107" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="D107" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0.9999999523809546</v>
+      </c>
     </row>
     <row r="108" ht="14.25" customHeight="1" s="8">
       <c r="A108" s="6" t="inlineStr">
@@ -4381,6 +4813,12 @@
       <c r="C108" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D108" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109" ht="14.25" customHeight="1" s="8">
       <c r="A109" s="6" t="inlineStr">
@@ -4396,6 +4834,12 @@
       <c r="C109" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="D109" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.9999998571428775</v>
+      </c>
     </row>
     <row r="110" ht="14.25" customHeight="1" s="8">
       <c r="A110" s="6" t="inlineStr">
@@ -4411,6 +4855,12 @@
       <c r="C110" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="D110" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0.7142856632653098</v>
+      </c>
     </row>
     <row r="111" ht="14.25" customHeight="1" s="8">
       <c r="A111" s="6" t="inlineStr">
@@ -4426,6 +4876,12 @@
       <c r="C111" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="D111" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.4999999583333368</v>
+      </c>
     </row>
     <row r="112" ht="14.25" customHeight="1" s="8">
       <c r="A112" s="6" t="inlineStr">
@@ -4441,6 +4897,12 @@
       <c r="C112" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="D112" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0.99999990000001</v>
+      </c>
     </row>
     <row r="113" ht="14.25" customHeight="1" s="8">
       <c r="A113" s="6" t="inlineStr">
@@ -4456,6 +4918,12 @@
       <c r="C113" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="D113" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.5555554938271674</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1" s="8">
       <c r="A114" s="6" t="inlineStr">
@@ -4471,6 +4939,12 @@
       <c r="C114" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="D114" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0.7777777489711944</v>
+      </c>
     </row>
     <row r="115" ht="14.25" customHeight="1" s="8">
       <c r="A115" s="6" t="inlineStr">
@@ -4486,6 +4960,12 @@
       <c r="C115" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D115" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E115" t="n">
+        <v>-0.3333332222222593</v>
+      </c>
     </row>
     <row r="116" ht="14.25" customHeight="1" s="8">
       <c r="A116" s="6" t="inlineStr">
@@ -4501,6 +4981,12 @@
       <c r="C116" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="D116" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.599999880000024</v>
+      </c>
     </row>
     <row r="117" ht="14.25" customHeight="1" s="8">
       <c r="A117" s="6" t="inlineStr">
@@ -4516,6 +5002,12 @@
       <c r="C117" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D117" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E117" t="n">
+        <v>-0.7499999062500118</v>
+      </c>
     </row>
     <row r="118" ht="14.25" customHeight="1" s="8">
       <c r="A118" s="6" t="inlineStr">
@@ -4531,6 +5023,12 @@
       <c r="C118" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="D118" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0.4166666493055562</v>
+      </c>
     </row>
     <row r="119" ht="14.25" customHeight="1" s="8">
       <c r="A119" s="6" t="inlineStr">
@@ -4546,6 +5044,12 @@
       <c r="C119" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="D119" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0.3333332962963004</v>
+      </c>
     </row>
     <row r="120" ht="14.25" customHeight="1" s="8">
       <c r="A120" s="6" t="inlineStr">
@@ -4561,6 +5065,12 @@
       <c r="C120" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121" ht="14.25" customHeight="1" s="8">
       <c r="A121" s="6" t="inlineStr">
@@ -4576,6 +5086,12 @@
       <c r="C121" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0.9999990000010001</v>
+      </c>
     </row>
     <row r="122" ht="14.25" customHeight="1" s="8">
       <c r="A122" s="6" t="inlineStr">
@@ -4591,6 +5107,12 @@
       <c r="C122" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="D122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0.9999998333333611</v>
+      </c>
     </row>
     <row r="123" ht="14.25" customHeight="1" s="8">
       <c r="A123" s="6" t="inlineStr">
@@ -4606,6 +5128,12 @@
       <c r="C123" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="D123" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0.1111110987654335</v>
+      </c>
     </row>
     <row r="124" ht="14.25" customHeight="1" s="8">
       <c r="A124" s="6" t="inlineStr">
@@ -4621,6 +5149,12 @@
       <c r="C124" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D124" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" ht="14.25" customHeight="1" s="8">
       <c r="A125" s="6" t="inlineStr">
@@ -4636,6 +5170,12 @@
       <c r="C125" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D125" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0.9999990000010001</v>
+      </c>
     </row>
     <row r="126" ht="14.25" customHeight="1" s="8">
       <c r="A126" s="6" t="inlineStr">
@@ -4651,6 +5191,12 @@
       <c r="C126" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="D126" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0.4117646816609011</v>
+      </c>
     </row>
     <row r="127" ht="14.25" customHeight="1" s="8">
       <c r="A127" s="6" t="inlineStr">
@@ -4666,6 +5212,12 @@
       <c r="C127" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D127" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0.99999950000025</v>
+      </c>
     </row>
     <row r="128" ht="14.25" customHeight="1" s="8">
       <c r="A128" s="6" t="inlineStr">
@@ -4681,6 +5233,12 @@
       <c r="C128" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D128" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E128" t="n">
+        <v>-0.4999999375000079</v>
+      </c>
     </row>
     <row r="129" ht="14.25" customHeight="1" s="8">
       <c r="A129" s="6" t="inlineStr">
@@ -4696,6 +5254,12 @@
       <c r="C129" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="D129" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E129" t="n">
+        <v>0.5555554938271674</v>
+      </c>
     </row>
     <row r="130" ht="14.25" customHeight="1" s="8">
       <c r="A130" s="6" t="inlineStr">
@@ -4711,6 +5275,12 @@
       <c r="C130" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="D130" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0.6666666111111158</v>
+      </c>
     </row>
     <row r="131" ht="14.25" customHeight="1" s="8">
       <c r="A131" s="6" t="inlineStr">
@@ -4726,6 +5296,12 @@
       <c r="C131" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="D131" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0.599999940000006</v>
+      </c>
     </row>
     <row r="132" ht="14.25" customHeight="1" s="8">
       <c r="A132" s="6" t="inlineStr">
@@ -4741,6 +5317,12 @@
       <c r="C132" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="D132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0.99999980000004</v>
+      </c>
     </row>
     <row r="133" ht="14.25" customHeight="1" s="8">
       <c r="A133" s="6" t="inlineStr">
@@ -4756,6 +5338,12 @@
       <c r="C133" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D133" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0.3333332222222593</v>
+      </c>
     </row>
     <row r="134" ht="14.25" customHeight="1" s="8">
       <c r="A134" s="6" t="inlineStr">
@@ -4771,6 +5359,12 @@
       <c r="C134" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="D134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0.9999997500000625</v>
+      </c>
     </row>
     <row r="135" ht="14.25" customHeight="1" s="8">
       <c r="A135" s="6" t="inlineStr">
@@ -4786,6 +5380,12 @@
       <c r="C135" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D135" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0.3333332222222593</v>
+      </c>
     </row>
     <row r="136" ht="14.25" customHeight="1" s="8">
       <c r="A136" s="6" t="inlineStr">
@@ -4801,6 +5401,12 @@
       <c r="C136" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D136" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E136" t="n">
+        <v>0.99999950000025</v>
+      </c>
     </row>
     <row r="137" ht="14.25" customHeight="1" s="8">
       <c r="A137" s="6" t="inlineStr">
@@ -4816,6 +5422,12 @@
       <c r="C137" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D137" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" t="n">
+        <v>0.99999950000025</v>
+      </c>
     </row>
     <row r="138" ht="14.25" customHeight="1" s="8">
       <c r="A138" s="6" t="inlineStr">
@@ -4831,6 +5443,12 @@
       <c r="C138" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D138" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E138" t="n">
+        <v>0.99999950000025</v>
+      </c>
     </row>
     <row r="139" ht="14.25" customHeight="1" s="8">
       <c r="A139" s="6" t="inlineStr">
@@ -4846,6 +5464,12 @@
       <c r="C139" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D139" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0.99999950000025</v>
+      </c>
     </row>
     <row r="140" ht="14.25" customHeight="1" s="8">
       <c r="A140" s="6" t="inlineStr">
@@ -4861,6 +5485,12 @@
       <c r="C140" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="D140" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0.9999997500000625</v>
+      </c>
     </row>
     <row r="141" ht="14.25" customHeight="1" s="8">
       <c r="A141" s="6" t="inlineStr">
@@ -4876,6 +5506,12 @@
       <c r="C141" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="D141" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0.7777776913580343</v>
+      </c>
     </row>
     <row r="142" ht="14.25" customHeight="1" s="8">
       <c r="A142" s="6" t="inlineStr">
@@ -4891,6 +5527,12 @@
       <c r="C142" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="D142" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E142" t="n">
+        <v>0.4666666355555577</v>
+      </c>
     </row>
     <row r="143" ht="14.25" customHeight="1" s="8">
       <c r="A143" s="6" t="inlineStr">
@@ -4906,6 +5548,12 @@
       <c r="C143" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="D143" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E143" t="n">
+        <v>-0.199999980000002</v>
+      </c>
     </row>
     <row r="144" ht="14.25" customHeight="1" s="8">
       <c r="A144" s="6" t="inlineStr">
@@ -4921,6 +5569,12 @@
       <c r="C144" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="D144" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E144" t="n">
+        <v>0.07692307100591762</v>
+      </c>
     </row>
     <row r="145" ht="14.25" customHeight="1" s="8">
       <c r="A145" s="6" t="inlineStr">
@@ -4936,6 +5590,12 @@
       <c r="C145" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="D145" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E145" t="n">
+        <v>0.2380952267573701</v>
+      </c>
     </row>
     <row r="146" ht="14.25" customHeight="1" s="8">
       <c r="A146" s="6" t="inlineStr">
@@ -4951,6 +5611,12 @@
       <c r="C146" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="D146" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E146" t="n">
+        <v>0.1764705778546719</v>
+      </c>
     </row>
     <row r="147" ht="14.25" customHeight="1" s="8">
       <c r="A147" s="6" t="inlineStr">
@@ -4966,6 +5632,12 @@
       <c r="C147" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D147" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148" ht="14.25" customHeight="1" s="8">
       <c r="A148" s="6" t="inlineStr">
@@ -4980,6 +5652,12 @@
       </c>
       <c r="C148" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D148" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E148" t="n">
+        <v>0.9999990000010001</v>
       </c>
     </row>
     <row r="149" ht="14.25" customHeight="1" s="8"/>

</xml_diff>